<commit_message>
añadir a los casos de prueba los resultados obtenidos
</commit_message>
<xml_diff>
--- a/test-cases/api-testcases(OK).xlsx
+++ b/test-cases/api-testcases(OK).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\OneDrive - SENA\Escritorio\Conocimientos Marithza\Testing\Proyectos\qa-projects-portfolio\src\test-cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\OneDrive - SENA\Escritorio\Conocimientos Marithza\Testing\Proyectos\qa-projects-portfolio\test-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9DAF1E-63DE-49C7-BD3D-70DBB3CFF414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4301AB-4B9D-4B2A-B252-CC31A471ADD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de pruebas" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,48 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="3">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="3">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
+  </valueMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -197,6 +239,80 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>2</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+  <rel r:id="rId3"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -464,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,7 +659,9 @@
       <c r="G3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="H3" s="4" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="I3" s="4" t="s">
         <v>11</v>
       </c>
@@ -568,7 +686,9 @@
       <c r="G4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="4"/>
+      <c r="H4" s="4" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="I4" s="4" t="s">
         <v>11</v>
       </c>
@@ -593,7 +713,9 @@
       <c r="G5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="4" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
       <c r="I5" s="4" t="s">
         <v>11</v>
       </c>

</xml_diff>